<commit_message>
Adjust load up settings
</commit_message>
<xml_diff>
--- a/SCL_Results.xlsx
+++ b/SCL_Results.xlsx
@@ -223,7 +223,7 @@
     <t>N, N, N, N, L, L, S, S, S, N, L, L, L, L, L, L, L, S, S, S, N, N, N, N</t>
   </si>
   <si>
-    <t>N, N, N, N, N, N, N, N, N, N, N, N, L, L, L, L, S, S, S, S, N, N, N, N</t>
+    <t>N, N, N, N, N, N, N, N, N, N, L, L, L, L, L, L, S, S, S, S, N, N, N, N</t>
   </si>
 </sst>
 </file>
@@ -1463,10 +1463,10 @@
         <v>0</v>
       </c>
       <c r="P27">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Q27">
-        <v>0.9666666666666667</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1495,10 +1495,10 @@
         <v>0</v>
       </c>
       <c r="P28">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q28">
-        <v>0.9625</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -1527,10 +1527,10 @@
         <v>0</v>
       </c>
       <c r="P29">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="Q29">
-        <v>0.7958333333333334</v>
+        <v>0.7708333333333334</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -1559,10 +1559,10 @@
         <v>0</v>
       </c>
       <c r="P30">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q30">
-        <v>0.7208333333333333</v>
+        <v>0.7125</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -1591,10 +1591,10 @@
         <v>0</v>
       </c>
       <c r="P31">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="Q31">
-        <v>0.6791666666666667</v>
+        <v>0.6083333333333334</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -1623,10 +1623,10 @@
         <v>0</v>
       </c>
       <c r="P32">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Q32">
-        <v>0.5833333333333333</v>
+        <v>0.5791666666666666</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -1655,10 +1655,10 @@
         <v>0</v>
       </c>
       <c r="P33">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q33">
-        <v>0.7333333333333334</v>
+        <v>0.7291666666666667</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -1975,10 +1975,10 @@
         <v>0</v>
       </c>
       <c r="P43">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="Q43">
-        <v>0.875</v>
+        <v>0.9458333333333333</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -2007,10 +2007,10 @@
         <v>0</v>
       </c>
       <c r="P44">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="Q44">
-        <v>0.4</v>
+        <v>0.4958333333333333</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -2039,10 +2039,10 @@
         <v>0</v>
       </c>
       <c r="P45">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="Q45">
-        <v>0.5208333333333333</v>
+        <v>0.5875</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -2071,10 +2071,10 @@
         <v>0</v>
       </c>
       <c r="P46">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q46">
-        <v>0.7791666666666667</v>
+        <v>0.7916666666666666</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -2103,10 +2103,10 @@
         <v>0</v>
       </c>
       <c r="P47">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="Q47">
-        <v>0.5916666666666667</v>
+        <v>0.6666666666666667</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -2135,10 +2135,10 @@
         <v>0</v>
       </c>
       <c r="P48">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q48">
-        <v>0.5166666666666666</v>
+        <v>0.4625</v>
       </c>
     </row>
     <row r="49" spans="1:17">
@@ -2167,10 +2167,10 @@
         <v>0</v>
       </c>
       <c r="P49">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="Q49">
-        <v>0.2916666666666666</v>
+        <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="50" spans="1:17">

</xml_diff>